<commit_message>
added DML data pt2
</commit_message>
<xml_diff>
--- a/data/Tables for Grant.xlsx
+++ b/data/Tables for Grant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcmedu-my.sharepoint.com/personal/u244834_bcm_edu/Documents/BCM/Projects/Gold Humanism Glasses Grant/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{844A9E27-7240-4912-A04E-54A685DDA6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{484E2D21-25BC-420C-970C-A6539EE9DC66}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{844A9E27-7240-4912-A04E-54A685DDA6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5828FC88-AEFC-4690-9954-57B17E440773}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{70097ACA-40E4-4859-8D7F-D73420E3B1DC}"/>
+    <workbookView xWindow="38280" yWindow="7275" windowWidth="29040" windowHeight="16440" xr2:uid="{70097ACA-40E4-4859-8D7F-D73420E3B1DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="151">
   <si>
     <t>18-29</t>
   </si>
@@ -365,131 +365,134 @@
     <t>Age Groups</t>
   </si>
   <si>
-    <t>14 (11.1)</t>
-  </si>
-  <si>
-    <t>73 (57.9)</t>
-  </si>
-  <si>
-    <t>32 (25.4)</t>
-  </si>
-  <si>
-    <t>7 (5.6)</t>
-  </si>
-  <si>
-    <t>16 (12.7)</t>
-  </si>
-  <si>
-    <t>110 (87.3)</t>
-  </si>
-  <si>
-    <t>1 (0.8)</t>
-  </si>
-  <si>
-    <t>101 (80.2)</t>
-  </si>
-  <si>
-    <t>11 (8.7)</t>
-  </si>
-  <si>
-    <t>8 (6.3)</t>
-  </si>
-  <si>
     <t>(Missing)</t>
   </si>
   <si>
-    <t>4 (3.2)</t>
-  </si>
-  <si>
-    <t>97 (77.0)</t>
-  </si>
-  <si>
-    <t>2 (1.6)</t>
-  </si>
-  <si>
     <t>County/City Health</t>
   </si>
   <si>
-    <t>25 (19.8)</t>
-  </si>
-  <si>
-    <t>34 (27.0)</t>
-  </si>
-  <si>
-    <t>23 (18.3)</t>
-  </si>
-  <si>
-    <t>27 (21.4)</t>
+    <t>Fear of Treatment</t>
+  </si>
+  <si>
+    <t>1 (0.7)</t>
+  </si>
+  <si>
+    <t>1 (0.4)</t>
   </si>
   <si>
     <t>Dia De La Mujer Latina
-(n = 126)</t>
-  </si>
-  <si>
-    <t>91 (63.6)</t>
-  </si>
-  <si>
-    <t>4 (2.8)</t>
-  </si>
-  <si>
-    <t>9 (6.3)</t>
-  </si>
-  <si>
-    <t>7 (4.9)</t>
-  </si>
-  <si>
-    <t>Fear of Treatment</t>
-  </si>
-  <si>
-    <t>1 (0.7)</t>
-  </si>
-  <si>
-    <t>11 (7.7)</t>
-  </si>
-  <si>
-    <t>24 (9.5)</t>
-  </si>
-  <si>
-    <t>53 (21.0)</t>
-  </si>
-  <si>
-    <t>33 (13.1)</t>
-  </si>
-  <si>
-    <t>37 (14.7)</t>
-  </si>
-  <si>
-    <t>34 (13.5)</t>
-  </si>
-  <si>
-    <t>22 (8.7)</t>
-  </si>
-  <si>
-    <t>40 (15.9)</t>
-  </si>
-  <si>
-    <t>9 (3.6)</t>
-  </si>
-  <si>
-    <t>17 (6.7)</t>
-  </si>
-  <si>
-    <t>36 (14.3)</t>
-  </si>
-  <si>
-    <t>35 (13.9)</t>
-  </si>
-  <si>
-    <t>41 (16.3)</t>
-  </si>
-  <si>
-    <t>70 (27.8)</t>
-  </si>
-  <si>
-    <t>1 (0.4)</t>
-  </si>
-  <si>
-    <t>16 (6.3)</t>
+(n = 134)</t>
+  </si>
+  <si>
+    <t>15 (11.2)</t>
+  </si>
+  <si>
+    <t>79 (59.0)</t>
+  </si>
+  <si>
+    <t>32 (23.9)</t>
+  </si>
+  <si>
+    <t>8 (6.0)</t>
+  </si>
+  <si>
+    <t>21 (15.7)</t>
+  </si>
+  <si>
+    <t>113 (84.3)</t>
+  </si>
+  <si>
+    <t>108 (80.6)</t>
+  </si>
+  <si>
+    <t>11 (8.2)</t>
+  </si>
+  <si>
+    <t>9 (6.7)</t>
+  </si>
+  <si>
+    <t>4 (3.0)</t>
+  </si>
+  <si>
+    <t>104 (77.6)</t>
+  </si>
+  <si>
+    <t>2 (1.5)</t>
+  </si>
+  <si>
+    <t>26 (19.4)</t>
+  </si>
+  <si>
+    <t>37 (27.6)</t>
+  </si>
+  <si>
+    <t>34 (25.4)</t>
+  </si>
+  <si>
+    <t>24 (17.9)</t>
+  </si>
+  <si>
+    <t>29 (21.6)</t>
+  </si>
+  <si>
+    <t>99 (63.5)</t>
+  </si>
+  <si>
+    <t>4 (2.6)</t>
+  </si>
+  <si>
+    <t>11 (7.1)</t>
+  </si>
+  <si>
+    <t>8 (5.1)</t>
+  </si>
+  <si>
+    <t>5 (3.2)</t>
+  </si>
+  <si>
+    <t>1 (0.6)</t>
+  </si>
+  <si>
+    <t>9 (5.8)</t>
+  </si>
+  <si>
+    <t>25 (9.3)</t>
+  </si>
+  <si>
+    <t>55 (20.5)</t>
+  </si>
+  <si>
+    <t>37 (13.8)</t>
+  </si>
+  <si>
+    <t>45 (16.8)</t>
+  </si>
+  <si>
+    <t>35 (13.1)</t>
+  </si>
+  <si>
+    <t>22 (8.2)</t>
+  </si>
+  <si>
+    <t>40 (14.9)</t>
+  </si>
+  <si>
+    <t>9 (3.4)</t>
+  </si>
+  <si>
+    <t>17 (6.3)</t>
+  </si>
+  <si>
+    <t>39 (14.6)</t>
+  </si>
+  <si>
+    <t>44 (16.4)</t>
+  </si>
+  <si>
+    <t>72 (26.9)</t>
+  </si>
+  <si>
+    <t>18 (6.7)</t>
   </si>
 </sst>
 </file>
@@ -940,9 +943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C62D45B-8923-4B5D-88BA-E3B5CE6F9E63}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -966,7 +967,7 @@
         <v>106</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -986,7 +987,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1004,7 +1005,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1022,7 +1023,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1040,7 +1041,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1060,7 +1061,7 @@
         <v>19</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1078,7 +1079,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1134,7 +1135,7 @@
         <v>14</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1152,7 +1153,7 @@
         <v>33</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1170,7 +1171,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1188,7 +1189,7 @@
         <v>14</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1206,13 +1207,13 @@
         <v>37</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>14</v>
@@ -1224,7 +1225,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1244,7 +1245,7 @@
         <v>42</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1262,7 +1263,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1304,7 +1305,7 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="7" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>14</v>
@@ -1316,7 +1317,7 @@
         <v>14</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1352,7 +1353,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1376,7 +1377,7 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>14</v>
@@ -1388,7 +1389,7 @@
         <v>3</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1426,7 +1427,7 @@
         <v>52</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1444,7 +1445,7 @@
         <v>52</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1462,7 +1463,7 @@
         <v>19</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1480,13 +1481,13 @@
         <v>56</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>14</v>
@@ -1498,7 +1499,7 @@
         <v>3</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1518,7 +1519,7 @@
         <v>61</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1536,7 +1537,7 @@
         <v>14</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1554,7 +1555,7 @@
         <v>14</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1572,7 +1573,7 @@
         <v>14</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1590,13 +1591,13 @@
         <v>14</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="7" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>14</v>
@@ -1608,7 +1609,7 @@
         <v>14</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1626,7 +1627,7 @@
         <v>3</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1644,13 +1645,13 @@
         <v>56</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>71</v>
@@ -1662,7 +1663,7 @@
         <v>61</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1682,7 +1683,7 @@
         <v>76</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1700,7 +1701,7 @@
         <v>79</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1718,7 +1719,7 @@
         <v>82</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1736,7 +1737,7 @@
         <v>85</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1754,7 +1755,7 @@
         <v>87</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1772,7 +1773,7 @@
         <v>89</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1790,7 +1791,7 @@
         <v>93</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1808,7 +1809,7 @@
         <v>14</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1828,7 +1829,7 @@
         <v>82</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1846,7 +1847,7 @@
         <v>100</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1882,7 +1883,7 @@
         <v>93</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1900,7 +1901,7 @@
         <v>87</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1918,7 +1919,7 @@
         <v>87</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1936,7 +1937,7 @@
         <v>87</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1954,7 +1955,7 @@
         <v>14</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>